<commit_message>
Warspirit Tower waves up to 145
</commit_message>
<xml_diff>
--- a/Theseus/Sketch.xlsx
+++ b/Theseus/Sketch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CTables\Wartune\Wartune\Theseus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB193920-0B79-4E1F-880B-4418D74314B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F62ED3-6F69-4230-B034-63DE5FD4A472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19318" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="19">
   <si>
     <t>Thunder Gust</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Non-boost (260)</t>
+  </si>
+  <si>
+    <t>Double-skill 4+5</t>
+  </si>
+  <si>
+    <t>Skill-auto n5 -&gt; a</t>
   </si>
 </sst>
 </file>
@@ -186,16 +192,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,15 +550,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L42"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="1" max="1" width="2.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
@@ -581,11 +587,11 @@
         <f>G1</f>
         <v>260</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -610,9 +616,9 @@
         <f>IF(OR(F1="Criminal Trial",F1="Lightning Nova"),G2*1.2,G2)</f>
         <v>260</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -907,26 +913,29 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="J16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K16" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
       <c r="B17" s="4" t="s">
         <v>0</v>
       </c>
@@ -956,7 +965,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -970,7 +979,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
       <c r="B19" s="4" t="s">
         <v>0</v>
       </c>
@@ -1000,21 +1012,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="6">
         <v>100</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
       <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
@@ -1023,7 +1038,7 @@
         <v>883</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D20:D41" si="2">IF(OR(B19="Criminal Trial",B19="Lightning Nova"),C21*1.2,C21)</f>
+        <f t="shared" ref="D21:D41" si="2">IF(OR(B19="Criminal Trial",B19="Lightning Nova"),C21*1.2,C21)</f>
         <v>883</v>
       </c>
       <c r="E21">
@@ -1044,7 +1059,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>10</v>
       </c>
@@ -1058,7 +1073,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
       <c r="B23" s="4" t="s">
         <v>0</v>
       </c>
@@ -1088,7 +1106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -1102,7 +1120,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
       <c r="B25" s="4" t="s">
         <v>1</v>
       </c>
@@ -1132,21 +1153,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="6">
         <v>100</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K26" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>6</v>
+      </c>
       <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
@@ -1182,7 +1206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>10</v>
       </c>
@@ -1196,7 +1220,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>7</v>
+      </c>
       <c r="B29" s="4" t="s">
         <v>0</v>
       </c>
@@ -1232,7 +1259,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>10</v>
       </c>
@@ -1246,7 +1273,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>8</v>
+      </c>
       <c r="B31" s="4" t="s">
         <v>1</v>
       </c>
@@ -1276,21 +1306,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="6">
         <v>100</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K32" s="8">
+      <c r="K32" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>9</v>
+      </c>
       <c r="B33" s="4" t="s">
         <v>2</v>
       </c>
@@ -1320,7 +1353,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>10</v>
       </c>
@@ -1334,7 +1367,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>10</v>
+      </c>
       <c r="B35" s="4" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1400,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>10</v>
       </c>
@@ -1378,7 +1414,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>11</v>
+      </c>
       <c r="B37" s="4" t="s">
         <v>1</v>
       </c>
@@ -1408,21 +1447,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="6">
         <v>100</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="H38" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K38" s="8">
+      <c r="K38" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12</v>
+      </c>
       <c r="B39" s="4" t="s">
         <v>3</v>
       </c>
@@ -1458,7 +1500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>10</v>
       </c>
@@ -1466,7 +1508,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>13</v>
+      </c>
       <c r="B41" s="4" t="s">
         <v>0</v>
       </c>
@@ -1496,7 +1541,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C42" s="4" t="s">
         <v>7</v>
       </c>
@@ -1512,9 +1557,29 @@
         <v>8974.1999999999989</v>
       </c>
     </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="J1:L2"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>